<commit_message>
Initial work on storing shared formulas.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-shared.xlsx
+++ b/test/xlsx/formula-shared.xlsx
@@ -342,15 +342,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1">
         <v>10</v>
       </c>
@@ -360,8 +360,34 @@
       <c r="D1">
         <v>11</v>
       </c>
+      <c r="E1">
+        <v>11</v>
+      </c>
+      <c r="G1">
+        <v>100</v>
+      </c>
+      <c r="H1">
+        <f>G1+2</f>
+        <v>102</v>
+      </c>
+      <c r="I1">
+        <f t="shared" ref="I1:L1" si="0">H1+2</f>
+        <v>104</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:12">
       <c r="A2">
         <f>A1+1</f>
         <v>11</v>
@@ -374,341 +400,77 @@
         <f>D1+1</f>
         <v>12</v>
       </c>
+      <c r="E2">
+        <f>E1+1</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:12">
       <c r="A3">
-        <f t="shared" ref="A3:B26" si="0">A2+1</f>
+        <f t="shared" ref="A3:B26" si="1">A2+1</f>
         <v>12</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3" si="1">D2+1</f>
+        <f t="shared" ref="D3:E3" si="2">D2+1</f>
         <v>13</v>
       </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:12">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4" si="2">D3+1</f>
+        <f t="shared" ref="D4:E4" si="3">D3+1</f>
         <v>14</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:12">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5" si="3">D4+1</f>
+        <f t="shared" ref="D5:E5" si="4">D4+1</f>
         <v>15</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:12">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6" si="4">D5+1</f>
+        <f t="shared" ref="D6:E6" si="5">D5+1</f>
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7" si="5">D6+1</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8" si="6">D7+1</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9" si="7">D8+1</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ref="D10" si="8">D9+1</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ref="D11" si="9">D10+1</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ref="D12" si="10">D11+1</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ref="D13" si="11">D12+1</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14" si="12">D13+1</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ref="D15" si="13">D14+1</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="D16">
-        <f t="shared" ref="D16" si="14">D15+1</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17" si="15">D16+1</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ref="D18" si="16">D17+1</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ref="D19" si="17">D18+1</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="D20">
-        <f t="shared" ref="D20" si="18">D19+1</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="D21">
-        <f t="shared" ref="D21" si="19">D20+1</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22" si="20">D21+1</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="D23">
-        <f t="shared" ref="D23" si="21">D22+1</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ref="D24" si="22">D23+1</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ref="D25" si="23">D24+1</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ref="D26" si="24">D25+1</f>
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>